<commit_message>
added new endpoints and refactor
</commit_message>
<xml_diff>
--- a/ReportService/ReportService/wwwroot/reports/12345678.xlsx
+++ b/ReportService/ReportService/wwwroot/reports/12345678.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Number</t>
   </si>
@@ -38,10 +38,19 @@
     <t>1</t>
   </si>
   <si>
+    <t>d2f89a58-4961-4fa3-baad-3f7eff79ce02</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>7/6/2024</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>80f17582-3156-49bd-b2ee-90ef9b5f9759</t>
-  </si>
-  <si>
-    <t>12345678</t>
   </si>
   <si>
     <t>7/5/2024</t>
@@ -101,7 +110,7 @@
   <sheetPr codeName="">
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -153,12 +162,35 @@
         <v>10</v>
       </c>
       <c r="E2" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0">
+        <v>5</v>
+      </c>
+      <c r="F3" s="0">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0">
         <v>5</v>
       </c>
     </row>

</xml_diff>